<commit_message>
many changes in design patterns, testing ! problems with referencing the plants (plants_sto)  dataframes
</commit_message>
<xml_diff>
--- a/Database/CapacityExpansion/techs_cost.xlsx
+++ b/Database/CapacityExpansion/techs_cost.xlsx
@@ -1,23 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-HP\Dropbox\Dispa-SET\Database\CapacityExpansion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421FA05-381C-4A05-96DE-E74B95AD6299}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1905" windowWidth="23835" windowHeight="12645" xr2:uid="{6194FD70-DB12-294C-9EAD-24922869828E}"/>
+    <workbookView xWindow="5160" yWindow="1905" windowWidth="23835" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="3" r:id="rId2"/>
-    <sheet name="Data_DIW88" sheetId="2" r:id="rId3"/>
+    <sheet name="csv_export" sheetId="1" r:id="rId1"/>
+    <sheet name="Data_DIW88" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>Unit</t>
   </si>
@@ -265,12 +258,6 @@
     <t>WTON</t>
   </si>
   <si>
-    <t>Lille</t>
-  </si>
-  <si>
-    <t>em</t>
-  </si>
-  <si>
     <t>WAT-HDAM</t>
   </si>
   <si>
@@ -295,29 +282,14 @@
     <t>WIN-WTON</t>
   </si>
   <si>
-    <t xml:space="preserve">nuclear	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lignite	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hardcoal	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ccgt	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ocgt	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">psp	</t>
+    <t xml:space="preserve">https://www.diw.de/documents/publikationen/73/diw_01.c.558112.de/diw_datadoc_2017-088.pdf </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,16 +322,18 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF98C379"/>
-      <name val="Monaco"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF98C379"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -403,8 +377,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -420,13 +395,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,56 +707,50 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30E8AA9-52D8-CD49-A9A7-21C91AFE90DF}">
-  <dimension ref="A1:O23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="19.125" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" t="s">
         <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1">
-        <v>2950000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -805,25 +775,8 @@
         <f>VLOOKUP($A2,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I2">
-        <f>E2/$E$5</f>
-        <v>9.166666666666666E-2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2">
-        <v>1700000</v>
-      </c>
-      <c r="N2">
-        <f>M2/$M$1</f>
-        <v>0.57627118644067798</v>
-      </c>
-      <c r="O2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -848,25 +801,8 @@
         <f>VLOOKUP($A3,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I14" si="0">E3/$E$5</f>
-        <v>0.3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3">
-        <v>1600000</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N6" si="1">M3/$M$1</f>
-        <v>0.5423728813559322</v>
-      </c>
-      <c r="O3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -891,22 +827,8 @@
         <f>VLOOKUP($A4,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4">
-        <v>750000</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="1"/>
-        <v>0.25423728813559321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -931,22 +853,8 @@
         <f>VLOOKUP($A5,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>91</v>
-      </c>
-      <c r="M5">
-        <v>650000</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="1"/>
-        <v>0.22033898305084745</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -971,35 +879,21 @@
         <f>VLOOKUP($A6,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="L6" t="s">
-        <v>92</v>
-      </c>
-      <c r="M6">
-        <v>750000</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
-        <v>0.25423728813559321</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f>VLOOKUP($A7,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>2000000</v>
       </c>
@@ -1007,29 +901,25 @@
         <f>VLOOKUP($A7,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>20000</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f>VLOOKUP($A7,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="13" t="s">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <f>VLOOKUP($A8,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>2000000</v>
       </c>
@@ -1037,29 +927,25 @@
         <f>VLOOKUP($A8,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>20000</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <f>VLOOKUP($A8,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="13" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f>VLOOKUP($A9,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>3000000</v>
       </c>
@@ -1067,29 +953,25 @@
         <f>VLOOKUP($A9,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>60000</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f>VLOOKUP($A9,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="13" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f>VLOOKUP($A10,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>998000</v>
       </c>
@@ -1097,29 +979,25 @@
         <f>VLOOKUP($A10,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>25000</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <f>VLOOKUP($A10,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0.16633333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="13" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <f>VLOOKUP($A11,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>2400000</v>
       </c>
@@ -1127,30 +1005,26 @@
         <f>VLOOKUP($A11,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>100000</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <f>VLOOKUP($A11,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="13" t="s">
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f>VLOOKUP($A12,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>2424000</v>
       </c>
@@ -1158,30 +1032,26 @@
         <f>VLOOKUP($A12,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>100000</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <f>VLOOKUP($A12,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>30</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="13" t="s">
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <f>VLOOKUP($A13,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>3500000</v>
       </c>
@@ -1189,30 +1059,26 @@
         <f>VLOOKUP($A13,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>35000</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <f>VLOOKUP($A13,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="13" t="s">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <f>VLOOKUP($A14,Data_DIW88!$A:$G,2,FALSE)*1000</f>
         <v>1063000</v>
       </c>
@@ -1220,47 +1086,43 @@
         <f>VLOOKUP($A14,Data_DIW88!$A:$G,3,FALSE)*1000</f>
         <v>35000</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f>VLOOKUP($A14,Data_DIW88!$A:$G,7,FALSE)</f>
         <v>20</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>0.17716666666666667</v>
-      </c>
-      <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="12:13">
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-    </row>
-    <row r="18" spans="12:13">
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-    </row>
-    <row r="19" spans="12:13">
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-    </row>
-    <row r="20" spans="12:13">
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-    </row>
-    <row r="21" spans="12:13">
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-    </row>
-    <row r="22" spans="12:13">
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="12:13">
-      <c r="L23" s="12"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1269,49 +1131,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3681F4EC-0C0C-485B-B6ED-A7CE53D1BEA1}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1">
-        <v>2016</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B8D830-E429-5441-92BB-0B68F0AEFBB1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C6:C14"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="2"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1319,7 +1157,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1342,12 +1180,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1370,7 +1208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +1231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1416,7 +1254,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1439,7 +1277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1462,7 +1300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1485,7 +1323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1508,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1531,7 +1369,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1554,7 +1392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -1577,7 +1415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
@@ -1600,7 +1438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
@@ -1623,7 +1461,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
@@ -1646,7 +1484,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1669,7 +1507,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -1692,7 +1530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
@@ -1738,7 +1576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
@@ -1761,7 +1599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
@@ -1784,7 +1622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
@@ -1807,7 +1645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>42</v>
       </c>
@@ -1830,7 +1668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>43</v>
       </c>
@@ -1853,7 +1691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>44</v>
       </c>
@@ -1876,7 +1714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>45</v>
       </c>
@@ -1899,7 +1737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>46</v>
       </c>
@@ -1922,7 +1760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>47</v>
       </c>
@@ -1948,7 +1786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>48</v>
       </c>
@@ -1974,7 +1812,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>49</v>
       </c>
@@ -2000,7 +1838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>50</v>
       </c>
@@ -2026,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>51</v>
       </c>
@@ -2052,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>52</v>
       </c>
@@ -2078,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
@@ -2104,52 +1942,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="10" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>